<commit_message>
properly saves to excel
</commit_message>
<xml_diff>
--- a/chat app 2/online_dataimporter/Excel.xlsx
+++ b/chat app 2/online_dataimporter/Excel.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Munka1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -385,10 +385,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -410,35 +410,252 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>43edg52</t>
+          <t>Sanguinaria canadensis</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Aquilegia canadensis</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>Caltha palustris</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>pingvin</t>
+          <t>Caltha palustris</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>43edg52</t>
+          <t>Dicentra cucullaria</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Asarum canadense</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Hepatica americana</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hepatica americana</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Arisaema triphyllum</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Podophyllum peltatum</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Phlox divaricata</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Phlox divaricata</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Claytonia Virginica</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Trillium grandiflorum</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Trillium grandiflorum</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Erythronium americanum</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Erythronium americanum</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Erythronium americanum</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Anemone blanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Anemone blanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Monarda didyma</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Monarda didyma</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Rudbeckia hirta</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Ranunculus</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ranunculus</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Asclepias tuberosa</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Potentilla</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Oenothera</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Gentiana</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Gentiana</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Polemonium caeruleum</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Polemonium caeruleum</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Eschscholzia californica</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Dodecatheon</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Cimicifuga</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Lobelia cardinalis</t>
         </is>
       </c>
     </row>

</xml_diff>